<commit_message>
Modify Timepoint col name in metadata
</commit_message>
<xml_diff>
--- a/metadata_input.xlsx
+++ b/metadata_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miniymay/Library/CloudStorage/GoogleDrive-joungminvt@gmail.com/My Drive/ciwars viz/testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miniymay/Library/CloudStorage/GoogleDrive-joungminvt@gmail.com/My Drive/ciwars viz/python script/ciwarsViz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B7C581C-F44E-3B45-A4FC-942FC6F385E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD57B8A-8338-7D40-977E-04C80DFB8D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6980" yWindow="3260" windowWidth="28100" windowHeight="17440"/>
+    <workbookView xWindow="700" yWindow="560" windowWidth="28100" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata_input" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <t>Sample Name</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>20-10-12</t>
   </si>
   <si>
@@ -107,12 +104,15 @@
   </si>
   <si>
     <t>l</t>
+  </si>
+  <si>
+    <t>Timepoint</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18">
     <font>
       <sz val="12"/>
@@ -929,11 +929,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -943,24 +943,24 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>7.05</v>
@@ -974,10 +974,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>8.18</v>
@@ -991,10 +991,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>4.91</v>
@@ -1008,10 +1008,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>3.31</v>
@@ -1025,10 +1025,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>2.68</v>
@@ -1042,10 +1042,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>3.18</v>
@@ -1059,10 +1059,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>5.65</v>
@@ -1076,10 +1076,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>7.05</v>
@@ -1093,10 +1093,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>8.18</v>
@@ -1110,10 +1110,10 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>4.91</v>
@@ -1127,10 +1127,10 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>3.31</v>
@@ -1144,10 +1144,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>2.68</v>

</xml_diff>

<commit_message>
Add the exception for metadata column containing strings
</commit_message>
<xml_diff>
--- a/metadata_input.xlsx
+++ b/metadata_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miniymay/Library/CloudStorage/GoogleDrive-joungminvt@gmail.com/My Drive/ciwars viz/python script/ciwarsViz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F85A57-4A2C-A049-8360-4E7CF3B8DCCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C726C3A-8C42-9847-9A9B-E5130E286126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="560" windowWidth="28100" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Sample Name</t>
   </si>
@@ -107,6 +107,18 @@
   </si>
   <si>
     <t>Time point</t>
+  </si>
+  <si>
+    <t>test column</t>
+  </si>
+  <si>
+    <t>test_a</t>
+  </si>
+  <si>
+    <t>test_b</t>
+  </si>
+  <si>
+    <t>test_c</t>
   </si>
 </sst>
 </file>
@@ -931,15 +943,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -955,8 +967,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -972,8 +987,11 @@
       <c r="E2">
         <v>11.8</v>
       </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -989,8 +1007,11 @@
       <c r="E3">
         <v>14</v>
       </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1006,8 +1027,11 @@
       <c r="E4">
         <v>20</v>
       </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1023,8 +1047,11 @@
       <c r="E5">
         <v>20.6</v>
       </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1040,8 +1067,11 @@
       <c r="E6">
         <v>22</v>
       </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1057,8 +1087,11 @@
       <c r="E7">
         <v>19.8</v>
       </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1074,8 +1107,11 @@
       <c r="E8">
         <v>14.1</v>
       </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1091,8 +1127,11 @@
       <c r="E9">
         <v>11.8</v>
       </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1108,8 +1147,11 @@
       <c r="E10">
         <v>14</v>
       </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1125,8 +1167,11 @@
       <c r="E11">
         <v>20</v>
       </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1142,8 +1187,11 @@
       <c r="E12">
         <v>20.6</v>
       </c>
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1158,6 +1206,9 @@
       </c>
       <c r="E13">
         <v>22</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>